<commit_message>
Change in the excel file.Please read it.
</commit_message>
<xml_diff>
--- a/Files_from_box/2020-04-09_CEU_Capstone_Econometric Model_inputs.xlsx
+++ b/Files_from_box/2020-04-09_CEU_Capstone_Econometric Model_inputs.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t xml:space="preserve">Input Name</t>
   </si>
@@ -51,7 +51,7 @@
     <t xml:space="preserve">Regulator consultations on future charging policy changes, including metering, renewable support etc</t>
   </si>
   <si>
-    <t xml:space="preserve">how to make a variable? Maybe use NLP?</t>
+    <t xml:space="preserve">how to make a variable? Maybe use NLP? \n Whic h links to use? How to interpret the data?</t>
   </si>
   <si>
     <t xml:space="preserve">National / regional government / tax authority tax charging announcements – current and future path</t>
@@ -69,10 +69,22 @@
     <t xml:space="preserve">TSO 10- years infrastructure development plans (usually available in several countries)</t>
   </si>
   <si>
+    <t xml:space="preserve">found one publication</t>
+  </si>
+  <si>
     <t xml:space="preserve">TSO/DSO  financial statements</t>
   </si>
   <si>
+    <t xml:space="preserve">There are financial statement, but what exactly to look for. /n https://sse.com/investors/reportsandresults/reports/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 years</t>
+  </si>
+  <si>
     <t xml:space="preserve">National energy demand forecasting (usually published by Energy regulator or TSOs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I could not find the repos for that</t>
   </si>
   <si>
     <t xml:space="preserve">National energy and Climate plans: Would be required in order to assess the Efficiency, RES, EV-CHARGING, ETC.. policies that may affect to green levies in the invoices</t>
@@ -322,14 +334,14 @@
   <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="7.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="33.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="1.44"/>
   </cols>
@@ -399,27 +411,44 @@
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D12" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" display="https://sse.com/investors/reportsandresults/reports/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -451,57 +480,57 @@
     <row r="1" customFormat="false" ht="5.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>